<commit_message>
update sample descriptive statistics file
</commit_message>
<xml_diff>
--- a/Sample descriptive statistics.xlsx
+++ b/Sample descriptive statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yimi/Desktop/Desktop Contents/Dissertation/Data Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74ECEED-60EE-9F49-ABDC-D6EC2D9F614B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F3BDA2-A639-6443-91CD-350CE61CBCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="620" windowWidth="47340" windowHeight="28180" xr2:uid="{A57578E6-31BD-C54B-9DD4-584B5A4E74C6}"/>
+    <workbookView xWindow="53120" yWindow="2460" windowWidth="47340" windowHeight="28180" xr2:uid="{A57578E6-31BD-C54B-9DD4-584B5A4E74C6}"/>
   </bookViews>
   <sheets>
     <sheet name="study 1_summary%" sheetId="2" r:id="rId1"/>
@@ -261,9 +261,6 @@
     <t>blank</t>
   </si>
   <si>
-    <t>STEM: 32,826; highest formal education: 33,124; occupation: 36, 687; job-related training: 38,493; work experience: 36,269; literacy/numeracy score: 38,541; PSTRE score: 30,079</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -371,6 +368,9 @@
   </si>
   <si>
     <t>STEM: 16,300; highest formal education: 18,559 ; occupation: 18,300; job-related training: 18,554; work experience: 17,978; literacy/numeracy score: 18, 570; PSTRE score: 14,468</t>
+  </si>
+  <si>
+    <t>STEM: 32,826; highest formal education: 38,533; occupation: 36, 687; job-related training: 38,493; work experience: 36,269; literacy/numeracy score: 38,541; PSTRE score: 30,079</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1499,7 @@
   <dimension ref="A2:X42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH28" sqref="AH28"/>
+      <selection activeCell="T55" sqref="T55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -2601,7 +2601,7 @@
         <v>276.14252966365279</v>
       </c>
       <c r="X13" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -3176,7 +3176,7 @@
         <v>264.72812495633218</v>
       </c>
       <c r="X19" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -4615,7 +4615,7 @@
         <v>255.55754507656371</v>
       </c>
       <c r="X34" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:24" ht="20" customHeight="1" x14ac:dyDescent="0.2">
@@ -5125,7 +5125,7 @@
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="75" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -5223,7 +5223,7 @@
         <v>66</v>
       </c>
       <c r="T2" s="160" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U2" s="162" t="s">
         <v>56</v>
@@ -7827,7 +7827,7 @@
     </row>
     <row r="33" spans="1:23" s="57" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="75"/>
       <c r="C33" s="82"/>
@@ -7876,7 +7876,7 @@
   <dimension ref="A2:AB40"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD42" sqref="AD42"/>
+      <selection activeCell="P56" sqref="P56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -11042,16 +11042,16 @@
         <f t="shared" si="0"/>
         <v>38493</v>
       </c>
-      <c r="Y40" s="141">
+      <c r="Y40" s="96">
         <v>36269</v>
       </c>
-      <c r="Z40" s="141">
-        <v>38541</v>
-      </c>
-      <c r="AA40" s="141">
-        <v>38541</v>
-      </c>
-      <c r="AB40" s="141">
+      <c r="Z40" s="96">
+        <v>38451</v>
+      </c>
+      <c r="AA40" s="96">
+        <v>38451</v>
+      </c>
+      <c r="AB40" s="96">
         <v>30079</v>
       </c>
     </row>
@@ -11095,37 +11095,37 @@
         <v>57</v>
       </c>
       <c r="B1" s="121" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="121" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="121" t="s">
+      <c r="D1" s="121" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="121" t="s">
+      <c r="E1" s="121" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="121" t="s">
+      <c r="F1" s="121" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="121" t="s">
+      <c r="G1" s="121" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="121" t="s">
+      <c r="H1" s="121" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="121" t="s">
+      <c r="I1" s="121" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="121" t="s">
+      <c r="J1" s="121" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="121" t="s">
+      <c r="K1" s="121" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="121" t="s">
-        <v>83</v>
-      </c>
       <c r="L1" s="124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -12456,7 +12456,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B36" s="117">
         <v>278.92878014008613</v>
@@ -12495,7 +12495,7 @@
     </row>
     <row r="37" spans="1:12" s="122" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B37" s="123">
         <v>272.66836665602756</v>
@@ -12543,37 +12543,37 @@
         <v>58</v>
       </c>
       <c r="B40" s="121" t="s">
+        <v>85</v>
+      </c>
+      <c r="C40" s="121" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="121" t="s">
+      <c r="D40" s="121" t="s">
         <v>87</v>
       </c>
-      <c r="D40" s="121" t="s">
+      <c r="E40" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="E40" s="121" t="s">
+      <c r="F40" s="121" t="s">
         <v>89</v>
       </c>
-      <c r="F40" s="121" t="s">
+      <c r="G40" s="121" t="s">
         <v>90</v>
       </c>
-      <c r="G40" s="121" t="s">
+      <c r="H40" s="121" t="s">
         <v>91</v>
       </c>
-      <c r="H40" s="121" t="s">
+      <c r="I40" s="121" t="s">
         <v>92</v>
       </c>
-      <c r="I40" s="121" t="s">
+      <c r="J40" s="121" t="s">
         <v>93</v>
       </c>
-      <c r="J40" s="121" t="s">
+      <c r="K40" s="121" t="s">
         <v>94</v>
       </c>
-      <c r="K40" s="121" t="s">
-        <v>95</v>
-      </c>
       <c r="L40" s="121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
@@ -13904,7 +13904,7 @@
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B75" s="117">
         <v>263.41979905172434</v>
@@ -13943,7 +13943,7 @@
     </row>
     <row r="76" spans="1:12" s="122" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B76" s="123">
         <v>268.19651462157481</v>
@@ -13991,37 +13991,37 @@
         <v>59</v>
       </c>
       <c r="B79" s="121" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" s="121" t="s">
         <v>96</v>
       </c>
-      <c r="C79" s="121" t="s">
+      <c r="D79" s="121" t="s">
         <v>97</v>
       </c>
-      <c r="D79" s="121" t="s">
+      <c r="E79" s="121" t="s">
         <v>98</v>
       </c>
-      <c r="E79" s="121" t="s">
+      <c r="F79" s="121" t="s">
         <v>99</v>
       </c>
-      <c r="F79" s="121" t="s">
+      <c r="G79" s="121" t="s">
         <v>100</v>
       </c>
-      <c r="G79" s="121" t="s">
+      <c r="H79" s="121" t="s">
         <v>101</v>
       </c>
-      <c r="H79" s="121" t="s">
+      <c r="I79" s="121" t="s">
         <v>102</v>
       </c>
-      <c r="I79" s="121" t="s">
+      <c r="J79" s="121" t="s">
         <v>103</v>
       </c>
-      <c r="J79" s="121" t="s">
+      <c r="K79" s="121" t="s">
         <v>104</v>
       </c>
-      <c r="K79" s="121" t="s">
+      <c r="L79" s="121" t="s">
         <v>105</v>
-      </c>
-      <c r="L79" s="121" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
@@ -14380,7 +14380,7 @@
         <v>11</v>
       </c>
       <c r="L89" s="126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.2">
@@ -14583,7 +14583,7 @@
         <v>17</v>
       </c>
       <c r="L95" s="126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.2">
@@ -15137,7 +15137,7 @@
         <v>32</v>
       </c>
       <c r="L110" s="126" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="111" spans="1:12" x14ac:dyDescent="0.2">
@@ -15259,7 +15259,7 @@
     </row>
     <row r="114" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A114" s="119" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B114" s="117">
         <v>285.39491838095233</v>
@@ -15298,7 +15298,7 @@
     </row>
     <row r="115" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A115" s="122" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B115" s="123">
         <v>286.10294681438876</v>
@@ -15419,7 +15419,7 @@
         <v>64</v>
       </c>
       <c r="X2" s="183" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="Y2" s="171" t="s">
         <v>56</v>
@@ -16133,7 +16133,7 @@
         <v>279.91727077738096</v>
       </c>
       <c r="AA11" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
@@ -16451,7 +16451,7 @@
         <v>268.17209262234036</v>
       </c>
       <c r="AA15" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
@@ -17478,7 +17478,7 @@
         <v>260.73255330428134</v>
       </c>
       <c r="AA28" s="18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:27" x14ac:dyDescent="0.2">
@@ -17714,7 +17714,7 @@
     </row>
     <row r="33" spans="1:23" s="57" customFormat="1" ht="14" x14ac:dyDescent="0.2">
       <c r="A33" s="75" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B33" s="75"/>
       <c r="C33" s="82"/>
@@ -17778,37 +17778,37 @@
         <v>57</v>
       </c>
       <c r="B2" s="137" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="137" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="137" t="s">
+      <c r="D2" s="137" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="137" t="s">
+      <c r="E2" s="137" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="137" t="s">
+      <c r="F2" s="137" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="137" t="s">
+      <c r="G2" s="137" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="137" t="s">
+      <c r="H2" s="137" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="137" t="s">
+      <c r="I2" s="137" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="137" t="s">
+      <c r="J2" s="137" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="137" t="s">
+      <c r="K2" s="137" t="s">
         <v>82</v>
       </c>
-      <c r="K2" s="137" t="s">
-        <v>83</v>
-      </c>
       <c r="L2" s="138" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -18827,7 +18827,7 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B29" s="135">
         <v>279.48071342918638</v>
@@ -18869,37 +18869,37 @@
         <v>58</v>
       </c>
       <c r="B32" s="137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C32" s="137" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="137" t="s">
+      <c r="D32" s="137" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="137" t="s">
+      <c r="E32" s="137" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="137" t="s">
+      <c r="F32" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="137" t="s">
+      <c r="G32" s="137" t="s">
         <v>90</v>
       </c>
-      <c r="G32" s="137" t="s">
+      <c r="H32" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="H32" s="137" t="s">
+      <c r="I32" s="137" t="s">
         <v>92</v>
       </c>
-      <c r="I32" s="137" t="s">
+      <c r="J32" s="137" t="s">
         <v>93</v>
       </c>
-      <c r="J32" s="137" t="s">
+      <c r="K32" s="137" t="s">
         <v>94</v>
       </c>
-      <c r="K32" s="137" t="s">
-        <v>95</v>
-      </c>
       <c r="L32" s="138" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
@@ -19918,7 +19918,7 @@
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B59" s="135">
         <v>274.74328948519144</v>
@@ -19960,37 +19960,37 @@
         <v>59</v>
       </c>
       <c r="B62" s="137" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" s="137" t="s">
         <v>96</v>
       </c>
-      <c r="C62" s="137" t="s">
+      <c r="D62" s="137" t="s">
         <v>97</v>
       </c>
-      <c r="D62" s="137" t="s">
+      <c r="E62" s="137" t="s">
         <v>98</v>
       </c>
-      <c r="E62" s="137" t="s">
+      <c r="F62" s="137" t="s">
         <v>99</v>
       </c>
-      <c r="F62" s="137" t="s">
+      <c r="G62" s="137" t="s">
         <v>100</v>
       </c>
-      <c r="G62" s="137" t="s">
+      <c r="H62" s="137" t="s">
         <v>101</v>
       </c>
-      <c r="H62" s="137" t="s">
+      <c r="I62" s="137" t="s">
         <v>102</v>
       </c>
-      <c r="I62" s="137" t="s">
+      <c r="J62" s="137" t="s">
         <v>103</v>
       </c>
-      <c r="J62" s="137" t="s">
+      <c r="K62" s="137" t="s">
         <v>104</v>
       </c>
-      <c r="K62" s="137" t="s">
+      <c r="L62" s="138" t="s">
         <v>105</v>
-      </c>
-      <c r="L62" s="138" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
@@ -21009,7 +21009,7 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="119" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B89" s="135">
         <v>289.45784266173581</v>

</xml_diff>